<commit_message>
Update notes on left square bracket
</commit_message>
<xml_diff>
--- a/Docs/PowerShell Special Character Escaping Techniques.xlsx
+++ b/Docs/PowerShell Special Character Escaping Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flesniak\Github\Repair-NTFSPermissions\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFDA7B8-3F95-404A-9C7C-480B06D8B79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98876B13-FB1C-42DC-829D-51070BBFBCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37020" yWindow="4590" windowWidth="27825" windowHeight="25320" xr2:uid="{1515D8EE-1A39-4837-8798-48B578DE46AF}"/>
+    <workbookView xWindow="38745" yWindow="7785" windowWidth="34890" windowHeight="19455" xr2:uid="{1515D8EE-1A39-4837-8798-48B578DE46AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
   <si>
     <t>Character</t>
   </si>
@@ -117,15 +117,6 @@
 2 (escape with grave accent)</t>
   </si>
   <si>
-    <t>2 (escape with grave accent)
-3 (escape with backslash)
-4 (regex escape)</t>
-  </si>
-  <si>
-    <t>3 (escape with backslash)
-4 (regex escape)</t>
-  </si>
-  <si>
     <t>{ (left curly brace)</t>
   </si>
   <si>
@@ -148,6 +139,15 @@
   </si>
   <si>
     <t>” (right curly double quotes, [char]8221)</t>
+  </si>
+  <si>
+    <t>[NOTHING WORKED]</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>To get ACL, escape with grave accent, then do Get-Item. Then, when the item is returned, access its method GetAccessControl()</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -222,9 +222,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,9 +536,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6EB366-3784-48AE-96A0-D4D060941C16}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -549,9 +551,10 @@
     <col min="2" max="2" width="24.875" customWidth="1"/>
     <col min="3" max="3" width="25.125" customWidth="1"/>
     <col min="4" max="4" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -564,8 +567,11 @@
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -578,8 +584,9 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -592,8 +599,9 @@
       <c r="D3" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -606,8 +614,9 @@
       <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -620,8 +629,9 @@
       <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -634,8 +644,9 @@
       <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -648,8 +659,9 @@
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -662,8 +674,9 @@
       <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -676,8 +689,9 @@
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -690,8 +704,9 @@
       <c r="D10" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -704,8 +719,9 @@
       <c r="D11" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -718,8 +734,9 @@
       <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
@@ -732,8 +749,9 @@
       <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -746,8 +764,9 @@
       <c r="D14" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
@@ -760,8 +779,9 @@
       <c r="D15" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -774,22 +794,26 @@
       <c r="D16" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+      <c r="E17" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -802,94 +826,101 @@
       <c r="D18" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>5</v>
@@ -900,10 +931,11 @@
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>34</v>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>5</v>
@@ -914,6 +946,7 @@
       <c r="D26" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix for square brackets in file names
</commit_message>
<xml_diff>
--- a/Docs/PowerShell Special Character Escaping Techniques.xlsx
+++ b/Docs/PowerShell Special Character Escaping Techniques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flesniak\Github\Repair-NTFSPermissions\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F754F2A-EBF5-4DA3-A5F3-8B87A9378D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F742B2-854C-4D4A-B23A-F4973D90D27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="11055" windowWidth="34890" windowHeight="19455" xr2:uid="{1515D8EE-1A39-4837-8798-48B578DE46AF}"/>
+    <workbookView xWindow="56370" yWindow="990" windowWidth="19110" windowHeight="18150" xr2:uid="{1515D8EE-1A39-4837-8798-48B578DE46AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,10 +148,12 @@
   </si>
   <si>
     <t>To get ACL, escape with grave accent, then do Get-Item. Then, when the item is returned, access its method GetAccessControl()
+Tested on PowerShell 1.0 on Windows Server 2008 SP1
 Tested on PowerShell 2.0 on Windows Server 2008 SP1</t>
   </si>
   <si>
-    <t>Tested on PowerShell 2.0 on Windows Server 2008 SP1</t>
+    <t>Tested on PowerShell 1.0 on Windows Server 2008 SP1
+Tested on PowerShell 2.0 on Windows Server 2008 SP1</t>
   </si>
 </sst>
 </file>
@@ -800,7 +802,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="99" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>